<commit_message>
kleine correctie gebied onbekend werkingsgebied woonmaatschappijen
</commit_message>
<xml_diff>
--- a/kerntabellen/gemeente_woonmaatschappij.xlsx
+++ b/kerntabellen/gemeente_woonmaatschappij.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\gebiedsniveaus\kerntabellen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F126D6-5969-43E9-9D16-FA3002ECD97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B38ED62-69CD-4D69-928C-2057A6BFB770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-4065" windowWidth="29040" windowHeight="15840" xr2:uid="{2F440909-EE07-4160-9ED3-7986FB46BC5D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2F440909-EE07-4160-9ED3-7986FB46BC5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -1082,16 +1082,16 @@
     <t>Buiten Vlaanderen en Brussel</t>
   </si>
   <si>
-    <t>Werkingsgebied woonmaatschappij onbekend (Vlaanderen)</t>
-  </si>
-  <si>
-    <t>Werkingsgebied woonmaatschappij onbekend (Brussel)</t>
-  </si>
-  <si>
     <t>name werkingsgebied_woonmaatschappij</t>
   </si>
   <si>
     <t>werkingsgebied_woonmaatschappij</t>
+  </si>
+  <si>
+    <t>Werkingsgebied onbekend (Vlaanderen)</t>
+  </si>
+  <si>
+    <t>Werkingsgebied onbekend (Brussel)</t>
   </si>
 </sst>
 </file>
@@ -1446,8 +1446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4690FC2-CCA2-405E-A37E-D829D18DB266}">
   <dimension ref="A1:D304"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A292" workbookViewId="0">
+      <selection activeCell="J305" sqref="J305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1460,10 +1460,10 @@
         <v>342</v>
       </c>
       <c r="C1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -5691,7 +5691,7 @@
         <v>91</v>
       </c>
       <c r="D303" s="1" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.3">
@@ -5705,7 +5705,7 @@
         <v>92</v>
       </c>
       <c r="D304" s="1" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>

</xml_diff>